<commit_message>
Move the dataset and models of emb2coord
</commit_message>
<xml_diff>
--- a/emb2coord.xlsx
+++ b/emb2coord.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\社交网络挖掘\POI\ours\snm-poi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093E5C31-E229-4FCE-9FB1-47887597FB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA54DDA-503B-4E85-A9DE-759BC1C28AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
   <si>
     <t>Key</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -189,6 +189,26 @@
   </si>
   <si>
     <t>LR0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EP130</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EP140</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(140,)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EP190</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(190,)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -525,7 +545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1321,10 +1341,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5673138E-F917-4D73-99CA-008F31016295}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1476,10 +1496,10 @@
         <v>37</v>
       </c>
       <c r="B6" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
-        <v>32</v>
+        <v>512</v>
       </c>
       <c r="D6" s="1">
         <v>128</v>
@@ -1505,13 +1525,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1">
-        <v>32</v>
+        <v>512</v>
       </c>
       <c r="D7" s="1">
         <v>128</v>
@@ -1536,10 +1556,68 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J8" s="2"/>
+      <c r="A8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>512</v>
+      </c>
+      <c r="D8" s="1">
+        <v>128</v>
+      </c>
+      <c r="E8" s="1">
+        <v>128</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="1">
+        <v>190</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J9" s="2"/>
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>512</v>
+      </c>
+      <c r="D9" s="1">
+        <v>128</v>
+      </c>
+      <c r="E9" s="1">
+        <v>128</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="1">
+        <v>140</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J10" s="2"/>
@@ -1585,6 +1663,9 @@
     </row>
     <row r="24" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J25" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>